<commit_message>
Add professionally formatted portfolio files with colors, borders, and styling
</commit_message>
<xml_diff>
--- a/Portfolio report_Investment_07.02.2026.xlsx
+++ b/Portfolio report_Investment_07.02.2026.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -51,8 +51,19 @@
       <color rgb="00FFFFFF"/>
       <sz val="14"/>
     </font>
+    <font>
+      <i val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <sz val="10"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill/>
     </fill>
@@ -101,8 +112,26 @@
         <bgColor rgb="00E2EFDA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7E6E6"/>
+        <bgColor rgb="00E7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4B084"/>
+        <bgColor rgb="00F4B084"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F1DCDB"/>
+        <bgColor rgb="00F1DCDB"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -124,11 +153,69 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="00000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="00000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -147,6 +234,51 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,7 +646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,200 +661,240 @@
     <col width="15" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="25" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">         Portfolio report: Investment</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18" customHeight="1">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>Report Generated: February 7, 2026</t>
         </is>
       </c>
     </row>
     <row r="3" ht="8" customHeight="1"/>
-    <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
+    <row r="4" ht="22" customHeight="1">
+      <c r="A4" s="12" t="inlineStr">
         <is>
           <t>KEY PERFORMANCE INDICATORS</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="18" customHeight="1">
-      <c r="A5" s="3" t="inlineStr">
+    <row r="5" ht="20" customHeight="1">
+      <c r="A5" s="13" t="inlineStr">
         <is>
           <t>Metric</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="13" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="C5" s="13" t="inlineStr">
         <is>
           <t>Details</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="4" t="inlineStr">
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="14" t="inlineStr">
         <is>
           <t>Portfolio Growth</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="15" t="inlineStr">
         <is>
           <t>$133,267.19</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C6" s="16" t="inlineStr">
         <is>
           <t>1017.86% increase</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="4" t="inlineStr">
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="14" t="inlineStr">
         <is>
           <t>Starting Value</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="15" t="inlineStr">
         <is>
           <t>$13,092.90</t>
         </is>
       </c>
-      <c r="C7" s="6" t="inlineStr">
+      <c r="C7" s="16" t="inlineStr">
         <is>
           <t>Mar 25</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="4" t="inlineStr">
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="14" t="inlineStr">
         <is>
           <t>Ending Value</t>
         </is>
       </c>
-      <c r="B8" s="5" t="inlineStr">
+      <c r="B8" s="15" t="inlineStr">
         <is>
           <t>$146,360.09</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr">
+      <c r="C8" s="16" t="inlineStr">
         <is>
           <t>February 2026</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="4" t="inlineStr">
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="14" t="inlineStr">
         <is>
           <t>Total Profit</t>
         </is>
       </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="B9" s="15" t="inlineStr">
         <is>
           <t>$10,752.31</t>
         </is>
       </c>
-      <c r="C9" s="6" t="inlineStr">
+      <c r="C9" s="16" t="inlineStr">
         <is>
           <t>Last 12 months</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="4" t="inlineStr">
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="14" t="inlineStr">
         <is>
           <t>Total Dividends</t>
         </is>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B10" s="15" t="inlineStr">
         <is>
           <t>$1,865.85</t>
         </is>
       </c>
-      <c r="C10" s="6" t="inlineStr">
+      <c r="C10" s="16" t="inlineStr">
         <is>
           <t>Cumulative</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="16" customHeight="1">
-      <c r="A11" s="4" t="inlineStr">
+    <row r="11" ht="18" customHeight="1">
+      <c r="A11" s="14" t="inlineStr">
         <is>
           <t>Average Monthly Return</t>
         </is>
       </c>
-      <c r="B11" s="5" t="inlineStr">
+      <c r="B11" s="15" t="inlineStr">
         <is>
           <t>$896.03</t>
         </is>
       </c>
-      <c r="C11" s="6" t="inlineStr">
+      <c r="C11" s="16" t="inlineStr">
         <is>
           <t>Per month average</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="16" customHeight="1">
-      <c r="A12" s="4" t="inlineStr">
+    <row r="12" ht="18" customHeight="1">
+      <c r="A12" s="14" t="inlineStr">
         <is>
           <t>Positive Months</t>
         </is>
       </c>
-      <c r="B12" s="5" t="inlineStr">
+      <c r="B12" s="15" t="inlineStr">
         <is>
           <t>10 of 12</t>
         </is>
       </c>
-      <c r="C12" s="6" t="inlineStr">
+      <c r="C12" s="16" t="inlineStr">
         <is>
           <t>83% win rate</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="16" customHeight="1">
-      <c r="A13" s="4" t="inlineStr">
+    <row r="13" ht="18" customHeight="1">
+      <c r="A13" s="14" t="inlineStr">
         <is>
           <t>Best Month</t>
         </is>
       </c>
-      <c r="B13" s="5" t="inlineStr">
+      <c r="B13" s="15" t="inlineStr">
         <is>
           <t>$3,113.81</t>
         </is>
       </c>
-      <c r="C13" s="6" t="inlineStr">
+      <c r="C13" s="16" t="inlineStr">
         <is>
           <t>Highest profit</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="16" customHeight="1">
-      <c r="A14" s="4" t="inlineStr">
+    <row r="14" ht="18" customHeight="1">
+      <c r="A14" s="14" t="inlineStr">
         <is>
           <t>Worst Month</t>
         </is>
       </c>
-      <c r="B14" s="5" t="inlineStr">
+      <c r="B14" s="15" t="inlineStr">
         <is>
           <t>$-766.35</t>
         </is>
       </c>
-      <c r="C14" s="6" t="inlineStr">
+      <c r="C14" s="16" t="inlineStr">
         <is>
           <t>Lowest profit</t>
         </is>
       </c>
     </row>
+    <row r="15" ht="8" customHeight="1"/>
+    <row r="16" ht="22" customHeight="1">
+      <c r="A16" s="12" t="n"/>
+    </row>
+    <row r="17" ht="20" customHeight="1">
+      <c r="A17" s="13" t="n"/>
+      <c r="B17" s="13" t="n"/>
+      <c r="C17" s="13" t="n"/>
+      <c r="D17" s="13" t="n"/>
+      <c r="E17" s="13" t="n"/>
+    </row>
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="17" t="n"/>
+      <c r="B18" s="18" t="n"/>
+      <c r="C18" s="18" t="n"/>
+      <c r="D18" s="18" t="n"/>
+      <c r="E18" s="18" t="n"/>
+    </row>
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="17" t="n"/>
+      <c r="B19" s="18" t="n"/>
+      <c r="C19" s="18" t="n"/>
+      <c r="D19" s="18" t="n"/>
+      <c r="E19" s="18" t="n"/>
+    </row>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="17" t="n"/>
+      <c r="B20" s="18" t="n"/>
+      <c r="C20" s="18" t="n"/>
+      <c r="D20" s="18" t="n"/>
+      <c r="E20" s="18" t="n"/>
+    </row>
+    <row r="21" ht="18" customHeight="1">
+      <c r="A21" s="19" t="n"/>
+      <c r="B21" s="19" t="n"/>
+      <c r="C21" s="19" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="19" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="A16:E16"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A4:E4"/>
   </mergeCells>
@@ -736,7 +908,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -759,83 +931,83 @@
     <col width="14" customWidth="1" min="13" max="13"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" customHeight="1">
-      <c r="A1" s="7" t="inlineStr">
+    <row r="1" ht="25" customHeight="1">
+      <c r="A1" s="20" t="inlineStr">
         <is>
           <t>MONTHLY PERFORMANCE ANALYSIS</t>
         </is>
       </c>
     </row>
     <row r="2" ht="8" customHeight="1"/>
-    <row r="3" ht="18" customHeight="1">
-      <c r="A3" s="3" t="inlineStr">
+    <row r="3" ht="22" customHeight="1">
+      <c r="A3" s="13" t="inlineStr">
         <is>
           <t>Period</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="13" t="inlineStr">
         <is>
           <t>Mar 25</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C3" s="13" t="inlineStr">
         <is>
           <t>Apr 25</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D3" s="13" t="inlineStr">
         <is>
           <t>May 25</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E3" s="13" t="inlineStr">
         <is>
           <t>Jun 25</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="13" t="inlineStr">
         <is>
           <t>Jul 25</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="G3" s="13" t="inlineStr">
         <is>
           <t>Aug 25</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="H3" s="13" t="inlineStr">
         <is>
           <t>Sep 25</t>
         </is>
       </c>
-      <c r="I3" s="3" t="inlineStr">
+      <c r="I3" s="13" t="inlineStr">
         <is>
           <t>Oct 25</t>
         </is>
       </c>
-      <c r="J3" s="3" t="inlineStr">
+      <c r="J3" s="13" t="inlineStr">
         <is>
           <t>Nov 25</t>
         </is>
       </c>
-      <c r="K3" s="3" t="inlineStr">
+      <c r="K3" s="13" t="inlineStr">
         <is>
           <t>Dec 25</t>
         </is>
       </c>
-      <c r="L3" s="3" t="inlineStr">
+      <c r="L3" s="13" t="inlineStr">
         <is>
           <t>Jan 26</t>
         </is>
       </c>
-      <c r="M3" s="3" t="inlineStr">
+      <c r="M3" s="13" t="inlineStr">
         <is>
           <t>Feb 26</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="4" ht="18" customHeight="1">
+      <c r="A4" s="21" t="inlineStr">
         <is>
           <t>Portfolio Value (Start)</t>
         </is>
@@ -877,8 +1049,8 @@
         <v>160147.61</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="21" t="inlineStr">
         <is>
           <t>Portfolio Value (End)</t>
         </is>
@@ -920,28 +1092,28 @@
         <v>146360.09</v>
       </c>
     </row>
-    <row r="6"/>
-    <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="4" t="inlineStr">
+    <row r="6" ht="8" customHeight="1"/>
+    <row r="7" ht="20" customHeight="1">
+      <c r="A7" s="22" t="inlineStr">
         <is>
           <t>PROFIT METRICS</t>
         </is>
       </c>
-      <c r="B7" s="8" t="n"/>
-      <c r="C7" s="8" t="n"/>
-      <c r="D7" s="8" t="n"/>
-      <c r="E7" s="8" t="n"/>
-      <c r="F7" s="8" t="n"/>
-      <c r="G7" s="8" t="n"/>
-      <c r="H7" s="8" t="n"/>
-      <c r="I7" s="8" t="n"/>
-      <c r="J7" s="8" t="n"/>
-      <c r="K7" s="8" t="n"/>
-      <c r="L7" s="8" t="n"/>
-      <c r="M7" s="8" t="n"/>
-    </row>
-    <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="B7" s="23" t="n"/>
+      <c r="C7" s="23" t="n"/>
+      <c r="D7" s="23" t="n"/>
+      <c r="E7" s="23" t="n"/>
+      <c r="F7" s="23" t="n"/>
+      <c r="G7" s="23" t="n"/>
+      <c r="H7" s="23" t="n"/>
+      <c r="I7" s="23" t="n"/>
+      <c r="J7" s="23" t="n"/>
+      <c r="K7" s="23" t="n"/>
+      <c r="L7" s="23" t="n"/>
+      <c r="M7" s="24" t="n"/>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="21" t="inlineStr">
         <is>
           <t>Total profit</t>
         </is>
@@ -983,8 +1155,8 @@
         <v>1212.48</v>
       </c>
     </row>
-    <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="4" t="inlineStr">
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="21" t="inlineStr">
         <is>
           <t>Total profit, %</t>
         </is>
@@ -1026,8 +1198,8 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="4" t="inlineStr">
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="21" t="inlineStr">
         <is>
           <t>Profit from price change</t>
         </is>
@@ -1069,8 +1241,8 @@
         <v>997.25</v>
       </c>
     </row>
-    <row r="11" ht="16" customHeight="1">
-      <c r="A11" s="4" t="inlineStr">
+    <row r="11" ht="18" customHeight="1">
+      <c r="A11" s="21" t="inlineStr">
         <is>
           <t>Net profit from sales</t>
         </is>
@@ -1120,8 +1292,8 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="16" customHeight="1">
-      <c r="A12" s="4" t="inlineStr">
+    <row r="12" ht="18" customHeight="1">
+      <c r="A12" s="21" t="inlineStr">
         <is>
           <t>Dividends</t>
         </is>
@@ -1163,28 +1335,28 @@
         <v>215.23</v>
       </c>
     </row>
-    <row r="13"/>
-    <row r="14" ht="18" customHeight="1">
-      <c r="A14" s="4" t="inlineStr">
+    <row r="13" ht="8" customHeight="1"/>
+    <row r="14" ht="20" customHeight="1">
+      <c r="A14" s="22" t="inlineStr">
         <is>
           <t>TRADING ACTIVITY</t>
         </is>
       </c>
-      <c r="B14" s="9" t="n"/>
-      <c r="C14" s="9" t="n"/>
-      <c r="D14" s="9" t="n"/>
-      <c r="E14" s="9" t="n"/>
-      <c r="F14" s="9" t="n"/>
-      <c r="G14" s="9" t="n"/>
-      <c r="H14" s="9" t="n"/>
-      <c r="I14" s="9" t="n"/>
-      <c r="J14" s="9" t="n"/>
-      <c r="K14" s="9" t="n"/>
-      <c r="L14" s="9" t="n"/>
-      <c r="M14" s="9" t="n"/>
-    </row>
-    <row r="15" ht="16" customHeight="1">
-      <c r="A15" s="4" t="inlineStr">
+      <c r="B14" s="23" t="n"/>
+      <c r="C14" s="23" t="n"/>
+      <c r="D14" s="23" t="n"/>
+      <c r="E14" s="23" t="n"/>
+      <c r="F14" s="23" t="n"/>
+      <c r="G14" s="23" t="n"/>
+      <c r="H14" s="23" t="n"/>
+      <c r="I14" s="23" t="n"/>
+      <c r="J14" s="23" t="n"/>
+      <c r="K14" s="23" t="n"/>
+      <c r="L14" s="23" t="n"/>
+      <c r="M14" s="24" t="n"/>
+    </row>
+    <row r="15" ht="18" customHeight="1">
+      <c r="A15" s="21" t="inlineStr">
         <is>
           <t>Total trades</t>
         </is>
@@ -1226,8 +1398,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" ht="16" customHeight="1">
-      <c r="A16" s="4" t="inlineStr">
+    <row r="16" ht="18" customHeight="1">
+      <c r="A16" s="21" t="inlineStr">
         <is>
           <t>Buy trades</t>
         </is>
@@ -1269,8 +1441,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" ht="16" customHeight="1">
-      <c r="A17" s="4" t="inlineStr">
+    <row r="17" ht="18" customHeight="1">
+      <c r="A17" s="21" t="inlineStr">
         <is>
           <t>Sell trades</t>
         </is>
@@ -1318,8 +1490,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" ht="16" customHeight="1">
-      <c r="A18" s="4" t="inlineStr">
+    <row r="18" ht="18" customHeight="1">
+      <c r="A18" s="21" t="inlineStr">
         <is>
           <t>Total purchases</t>
         </is>
@@ -1361,8 +1533,8 @@
         <v>215.23</v>
       </c>
     </row>
-    <row r="19" ht="16" customHeight="1">
-      <c r="A19" s="4" t="inlineStr">
+    <row r="19" ht="18" customHeight="1">
+      <c r="A19" s="21" t="inlineStr">
         <is>
           <t>Total sales</t>
         </is>
@@ -1410,10 +1582,125 @@
         <v>15000</v>
       </c>
     </row>
+    <row r="20" ht="18" customHeight="1">
+      <c r="A20" s="21" t="n"/>
+      <c r="B20" s="9" t="n"/>
+      <c r="C20" s="9" t="n"/>
+      <c r="D20" s="9" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+      <c r="G20" s="9" t="n"/>
+      <c r="H20" s="9" t="n"/>
+      <c r="I20" s="9" t="n"/>
+      <c r="J20" s="9" t="n"/>
+      <c r="K20" s="9" t="n"/>
+      <c r="L20" s="9" t="n"/>
+      <c r="M20" s="9" t="n"/>
+    </row>
+    <row r="21" ht="8" customHeight="1"/>
+    <row r="22" ht="20" customHeight="1">
+      <c r="A22" s="12" t="n"/>
+    </row>
+    <row r="23" ht="18" customHeight="1">
+      <c r="A23" s="21" t="n"/>
+      <c r="B23" s="25" t="n"/>
+      <c r="C23" s="25" t="n"/>
+      <c r="D23" s="25" t="n"/>
+      <c r="E23" s="25" t="n"/>
+      <c r="F23" s="25" t="n"/>
+      <c r="G23" s="25" t="n"/>
+      <c r="H23" s="25" t="n"/>
+      <c r="I23" s="25" t="n"/>
+      <c r="J23" s="25" t="n"/>
+      <c r="K23" s="25" t="n"/>
+      <c r="L23" s="25" t="n"/>
+      <c r="M23" s="25" t="n"/>
+    </row>
+    <row r="24" ht="18" customHeight="1">
+      <c r="A24" s="21" t="n"/>
+      <c r="B24" s="25" t="n"/>
+      <c r="C24" s="25" t="n"/>
+      <c r="D24" s="25" t="n"/>
+      <c r="E24" s="25" t="n"/>
+      <c r="F24" s="25" t="n"/>
+      <c r="G24" s="25" t="n"/>
+      <c r="H24" s="25" t="n"/>
+      <c r="I24" s="25" t="n"/>
+      <c r="J24" s="25" t="n"/>
+      <c r="K24" s="25" t="n"/>
+      <c r="L24" s="25" t="n"/>
+      <c r="M24" s="25" t="n"/>
+    </row>
+    <row r="25" ht="18" customHeight="1">
+      <c r="A25" s="21" t="n"/>
+      <c r="B25" s="25" t="n"/>
+      <c r="C25" s="25" t="n"/>
+      <c r="D25" s="25" t="n"/>
+      <c r="E25" s="25" t="n"/>
+      <c r="F25" s="25" t="n"/>
+      <c r="G25" s="25" t="n"/>
+      <c r="H25" s="25" t="n"/>
+      <c r="I25" s="25" t="n"/>
+      <c r="J25" s="25" t="n"/>
+      <c r="K25" s="25" t="n"/>
+      <c r="L25" s="25" t="n"/>
+      <c r="M25" s="25" t="n"/>
+    </row>
+    <row r="26" ht="8" customHeight="1"/>
+    <row r="27" ht="20" customHeight="1">
+      <c r="A27" s="12" t="n"/>
+    </row>
+    <row r="28" ht="18" customHeight="1">
+      <c r="A28" s="21" t="n"/>
+      <c r="B28" s="26" t="n"/>
+      <c r="C28" s="26" t="n"/>
+      <c r="D28" s="26" t="n"/>
+      <c r="E28" s="26" t="n"/>
+      <c r="F28" s="26" t="n"/>
+      <c r="G28" s="26" t="n"/>
+      <c r="H28" s="26" t="n"/>
+      <c r="I28" s="26" t="n"/>
+      <c r="J28" s="26" t="n"/>
+      <c r="K28" s="26" t="n"/>
+      <c r="L28" s="26" t="n"/>
+      <c r="M28" s="26" t="n"/>
+    </row>
+    <row r="29" ht="18" customHeight="1">
+      <c r="A29" s="21" t="n"/>
+      <c r="B29" s="26" t="n"/>
+      <c r="C29" s="26" t="n"/>
+      <c r="D29" s="26" t="n"/>
+      <c r="E29" s="26" t="n"/>
+      <c r="F29" s="26" t="n"/>
+      <c r="G29" s="26" t="n"/>
+      <c r="H29" s="26" t="n"/>
+      <c r="I29" s="26" t="n"/>
+      <c r="J29" s="26" t="n"/>
+      <c r="K29" s="26" t="n"/>
+      <c r="L29" s="26" t="n"/>
+      <c r="M29" s="26" t="n"/>
+    </row>
+    <row r="30" ht="18" customHeight="1">
+      <c r="A30" s="21" t="n"/>
+      <c r="B30" s="26" t="n"/>
+      <c r="C30" s="26" t="n"/>
+      <c r="D30" s="26" t="n"/>
+      <c r="E30" s="26" t="n"/>
+      <c r="F30" s="26" t="n"/>
+      <c r="G30" s="26" t="n"/>
+      <c r="H30" s="26" t="n"/>
+      <c r="I30" s="26" t="n"/>
+      <c r="J30" s="26" t="n"/>
+      <c r="K30" s="26" t="n"/>
+      <c r="L30" s="26" t="n"/>
+      <c r="M30" s="26" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A14:M14"/>
     <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="A22:M22"/>
     <mergeCell ref="A7:M7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1448,8 +1735,6 @@
         </is>
       </c>
     </row>
-    <row r="3"/>
-    <row r="4"/>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
@@ -1684,7 +1969,6 @@
         <v>-13787.52</v>
       </c>
     </row>
-    <row r="10"/>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
@@ -2158,7 +2442,6 @@
         </is>
       </c>
     </row>
-    <row r="20"/>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
@@ -2294,7 +2577,6 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="24"/>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
@@ -2430,7 +2712,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28"/>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
@@ -2631,8 +2912,6 @@
         </is>
       </c>
     </row>
-    <row r="33"/>
-    <row r="34"/>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Fix formatting on restructured portfolio files - complete professional styling
</commit_message>
<xml_diff>
--- a/Portfolio report_Investment_07.02.2026.xlsx
+++ b/Portfolio report_Investment_07.02.2026.xlsx
@@ -908,7 +908,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -916,7 +916,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="28" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
@@ -1646,24 +1646,38 @@
       <c r="L25" s="25" t="n"/>
       <c r="M25" s="25" t="n"/>
     </row>
-    <row r="26" ht="8" customHeight="1"/>
-    <row r="27" ht="20" customHeight="1">
+    <row r="26" ht="18" customHeight="1">
+      <c r="A26" s="21" t="n"/>
+      <c r="B26" s="25" t="n"/>
+      <c r="C26" s="25" t="n"/>
+      <c r="D26" s="25" t="n"/>
+      <c r="E26" s="25" t="n"/>
+      <c r="F26" s="25" t="n"/>
+      <c r="G26" s="25" t="n"/>
+      <c r="H26" s="25" t="n"/>
+      <c r="I26" s="25" t="n"/>
+      <c r="J26" s="25" t="n"/>
+      <c r="K26" s="25" t="n"/>
+      <c r="L26" s="25" t="n"/>
+      <c r="M26" s="25" t="n"/>
+    </row>
+    <row r="27" ht="8" customHeight="1">
       <c r="A27" s="12" t="n"/>
     </row>
-    <row r="28" ht="18" customHeight="1">
-      <c r="A28" s="21" t="n"/>
-      <c r="B28" s="26" t="n"/>
-      <c r="C28" s="26" t="n"/>
-      <c r="D28" s="26" t="n"/>
-      <c r="E28" s="26" t="n"/>
-      <c r="F28" s="26" t="n"/>
-      <c r="G28" s="26" t="n"/>
-      <c r="H28" s="26" t="n"/>
-      <c r="I28" s="26" t="n"/>
-      <c r="J28" s="26" t="n"/>
-      <c r="K28" s="26" t="n"/>
-      <c r="L28" s="26" t="n"/>
-      <c r="M28" s="26" t="n"/>
+    <row r="28" ht="20" customHeight="1">
+      <c r="A28" s="22" t="n"/>
+      <c r="B28" s="23" t="n"/>
+      <c r="C28" s="23" t="n"/>
+      <c r="D28" s="23" t="n"/>
+      <c r="E28" s="23" t="n"/>
+      <c r="F28" s="23" t="n"/>
+      <c r="G28" s="23" t="n"/>
+      <c r="H28" s="23" t="n"/>
+      <c r="I28" s="23" t="n"/>
+      <c r="J28" s="23" t="n"/>
+      <c r="K28" s="23" t="n"/>
+      <c r="L28" s="23" t="n"/>
+      <c r="M28" s="24" t="n"/>
     </row>
     <row r="29" ht="18" customHeight="1">
       <c r="A29" s="21" t="n"/>
@@ -1695,13 +1709,44 @@
       <c r="L30" s="26" t="n"/>
       <c r="M30" s="26" t="n"/>
     </row>
+    <row r="31" ht="18" customHeight="1">
+      <c r="A31" s="21" t="n"/>
+      <c r="B31" s="26" t="n"/>
+      <c r="C31" s="26" t="n"/>
+      <c r="D31" s="26" t="n"/>
+      <c r="E31" s="26" t="n"/>
+      <c r="F31" s="26" t="n"/>
+      <c r="G31" s="26" t="n"/>
+      <c r="H31" s="26" t="n"/>
+      <c r="I31" s="26" t="n"/>
+      <c r="J31" s="26" t="n"/>
+      <c r="K31" s="26" t="n"/>
+      <c r="L31" s="26" t="n"/>
+      <c r="M31" s="26" t="n"/>
+    </row>
+    <row r="32" ht="18" customHeight="1">
+      <c r="A32" s="21" t="n"/>
+      <c r="B32" s="26" t="n"/>
+      <c r="C32" s="26" t="n"/>
+      <c r="D32" s="26" t="n"/>
+      <c r="E32" s="26" t="n"/>
+      <c r="F32" s="26" t="n"/>
+      <c r="G32" s="26" t="n"/>
+      <c r="H32" s="26" t="n"/>
+      <c r="I32" s="26" t="n"/>
+      <c r="J32" s="26" t="n"/>
+      <c r="K32" s="26" t="n"/>
+      <c r="L32" s="26" t="n"/>
+      <c r="M32" s="26" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A14:M14"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A27:M27"/>
     <mergeCell ref="A22:M22"/>
     <mergeCell ref="A7:M7"/>
+    <mergeCell ref="A28:M28"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>